<commit_message>
Tech updates, new Overview sheet
</commit_message>
<xml_diff>
--- a/$RDDT.xlsx
+++ b/$RDDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246B3ABB-5228-47F4-9211-17EA493CFFC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F483239A-E7DD-45A6-A32E-8794908CFE5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27885" windowHeight="11340" activeTab="1" xr2:uid="{67A8AEE5-5541-4C98-BDDF-E609681A57BD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27885" windowHeight="11340" xr2:uid="{67A8AEE5-5541-4C98-BDDF-E609681A57BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="115">
   <si>
     <t>$RDDT</t>
   </si>
@@ -184,9 +184,6 @@
     <t>Q123</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Balance Sheet</t>
   </si>
   <si>
@@ -350,6 +347,30 @@
   </si>
   <si>
     <t>FY34</t>
+  </si>
+  <si>
+    <t>FCF TTM</t>
+  </si>
+  <si>
+    <t>FCF per share</t>
+  </si>
+  <si>
+    <t>P/FCF</t>
+  </si>
+  <si>
+    <t>Emply.</t>
+  </si>
+  <si>
+    <t>Headcount</t>
+  </si>
+  <si>
+    <t>Headcount Y/Y</t>
+  </si>
+  <si>
+    <t>FY22</t>
+  </si>
+  <si>
+    <t>FY21</t>
   </si>
 </sst>
 </file>
@@ -360,7 +381,7 @@
     <numFmt numFmtId="164" formatCode="mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,25 +447,6 @@
       <i/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="4"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -568,7 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -644,51 +646,52 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -768,6 +771,61 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95C8680D-9552-4A89-927E-7FA7A9FC4547}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5734050" y="9525"/>
+          <a:ext cx="0" cy="14468475"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1072,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C75DF7-9041-4171-92CA-8771AF69EB10}">
   <dimension ref="A2:W41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1111,19 +1169,19 @@
       <c r="M5" s="51"/>
       <c r="N5" s="51"/>
       <c r="O5" s="52"/>
-      <c r="T5" s="43" t="s">
-        <v>82</v>
-      </c>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="43"/>
+      <c r="T5" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="U5" s="55"/>
+      <c r="V5" s="55"/>
+      <c r="W5" s="55"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="2">
-        <v>78.599999999999994</v>
+        <v>116.05</v>
       </c>
       <c r="D6" s="29"/>
       <c r="G6" s="13"/>
@@ -1136,7 +1194,7 @@
       <c r="N6" s="7"/>
       <c r="O6" s="8"/>
       <c r="T6" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
@@ -1147,11 +1205,12 @@
         <v>4</v>
       </c>
       <c r="C7" s="15">
-        <v>94.955523999999997</v>
+        <f>+'Financial Model'!I16</f>
+        <v>169.16992200000001</v>
       </c>
       <c r="D7" s="29" t="str">
         <f>+$C$32</f>
-        <v>Q224</v>
+        <v>Q324</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="7"/>
@@ -1163,7 +1222,7 @@
       <c r="N7" s="7"/>
       <c r="O7" s="8"/>
       <c r="T7" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
@@ -1175,7 +1234,7 @@
       </c>
       <c r="C8" s="15">
         <f>C6*C7</f>
-        <v>7463.5041863999995</v>
+        <v>19632.169448100001</v>
       </c>
       <c r="D8" s="29"/>
       <c r="G8" s="13"/>
@@ -1197,12 +1256,12 @@
         <v>6</v>
       </c>
       <c r="C9" s="15">
-        <f>+'Financial Model'!H60</f>
-        <v>1699.0509999999999</v>
+        <f>+'Financial Model'!I62</f>
+        <v>1744.9669999999999</v>
       </c>
       <c r="D9" s="29" t="str">
         <f t="shared" ref="D9:D11" si="0">+$C$32</f>
-        <v>Q224</v>
+        <v>Q324</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="7"/>
@@ -1223,12 +1282,12 @@
         <v>7</v>
       </c>
       <c r="C10" s="15">
-        <f>+'Financial Model'!H61</f>
+        <f>+'Financial Model'!I63</f>
         <v>0</v>
       </c>
       <c r="D10" s="29" t="str">
         <f t="shared" si="0"/>
-        <v>Q224</v>
+        <v>Q324</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="7"/>
@@ -1250,11 +1309,11 @@
       </c>
       <c r="C11" s="15">
         <f>C9-C10</f>
-        <v>1699.0509999999999</v>
+        <v>1744.9669999999999</v>
       </c>
       <c r="D11" s="29" t="str">
         <f t="shared" si="0"/>
-        <v>Q224</v>
+        <v>Q324</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="7"/>
@@ -1276,7 +1335,7 @@
       </c>
       <c r="C12" s="16">
         <f>C8-C11</f>
-        <v>5764.4531864</v>
+        <v>17887.202448100001</v>
       </c>
       <c r="D12" s="30"/>
       <c r="G12" s="13"/>
@@ -1344,10 +1403,10 @@
         <v>42186</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="47"/>
       <c r="G16" s="13"/>
@@ -1362,7 +1421,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B17" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="46"/>
       <c r="D17" s="47"/>
@@ -1370,7 +1429,7 @@
         <v>41275</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -1382,7 +1441,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B18" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" s="46"/>
       <c r="D18" s="47"/>
@@ -1398,7 +1457,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B19" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="46"/>
       <c r="D19" s="47"/>
@@ -1414,12 +1473,12 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B20" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="49"/>
+        <v>77</v>
+      </c>
+      <c r="C20" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="54"/>
       <c r="G20" s="36"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -1476,20 +1535,25 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="46">
-        <f>+'Financial Model'!H28</f>
-        <v>91.2</v>
+      <c r="C29" s="57">
+        <f>+'Financial Model'!I28</f>
+        <v>97.2</v>
       </c>
       <c r="D29" s="47"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B30" s="13"/>
-      <c r="C30" s="46"/>
+      <c r="B30" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="57">
+        <f>+'Financial Model'!O33</f>
+        <v>2013</v>
+      </c>
       <c r="D30" s="47"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
@@ -1502,21 +1566,20 @@
         <v>14</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D32" s="32">
-        <f>+'Financial Model'!H3</f>
-        <v>45510</v>
+        <v>45594</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="D33" s="55"/>
+      <c r="C33" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="49"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="50" t="s">
@@ -1530,8 +1593,8 @@
         <v>19</v>
       </c>
       <c r="C37" s="44">
-        <f>+C6/'Financial Model'!H58</f>
-        <v>6.8223911003862527</v>
+        <f>+C6/'Financial Model'!I60</f>
+        <v>9.9272299910295665</v>
       </c>
       <c r="D37" s="45"/>
     </row>
@@ -1565,6 +1628,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
@@ -1581,15 +1653,6 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C33:D33" r:id="rId1" display="Link" xr:uid="{F82EFD67-97F9-4AD3-AEF6-2D6984AA7CF2}"/>
@@ -1602,25 +1665,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A86E61-85C1-478D-A3A1-0D08F166CC45}">
-  <dimension ref="B1:Z73"/>
+  <dimension ref="B1:Z79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O16" sqref="O16"/>
+      <selection pane="bottomRight" activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="1"/>
-    <col min="5" max="6" width="9.140625" style="57"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" s="20" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:26" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C1" s="20" t="s">
         <v>51</v>
       </c>
@@ -1639,50 +1700,56 @@
       <c r="H1" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="21" t="s">
         <v>49</v>
       </c>
       <c r="J1" s="20" t="s">
         <v>50</v>
       </c>
+      <c r="M1" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>113</v>
+      </c>
       <c r="O1" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="Q1" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="R1" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="S1" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="T1" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="U1" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="V1" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="V1" s="20" t="s">
+      <c r="W1" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="W1" s="20" t="s">
+      <c r="X1" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="X1" s="20" t="s">
+      <c r="Y1" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="Y1" s="20" t="s">
+      <c r="Z1" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="Z1" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="2:26" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="2:26" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="18"/>
       <c r="C2" s="19">
         <v>45016</v>
@@ -1699,8 +1766,11 @@
       <c r="H2" s="19">
         <v>45473</v>
       </c>
-    </row>
-    <row r="3" spans="2:26" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I2" s="19">
+        <v>45565</v>
+      </c>
+    </row>
+    <row r="3" spans="2:26" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="18"/>
       <c r="G3" s="31">
         <v>45419</v>
@@ -1708,8 +1778,11 @@
       <c r="H3" s="31">
         <v>45510</v>
       </c>
-    </row>
-    <row r="4" spans="2:26" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="I3" s="31">
+        <v>45594</v>
+      </c>
+    </row>
+    <row r="4" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>28</v>
       </c>
@@ -1720,8 +1793,9 @@
       <c r="D4" s="23">
         <v>183.03100000000001</v>
       </c>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
+      <c r="E4" s="23">
+        <v>207.50800000000001</v>
+      </c>
       <c r="G4" s="23">
         <f>524.147-H4</f>
         <v>242.96300000000002</v>
@@ -1729,6 +1803,9 @@
       <c r="H4" s="23">
         <v>281.18400000000003</v>
       </c>
+      <c r="I4" s="23">
+        <v>348.351</v>
+      </c>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
@@ -1741,6 +1818,9 @@
       <c r="D5" s="24">
         <v>28.835999999999999</v>
       </c>
+      <c r="E5" s="24">
+        <v>26.395</v>
+      </c>
       <c r="G5" s="24">
         <f>57.117-H5</f>
         <v>27.615999999999996</v>
@@ -1748,8 +1828,11 @@
       <c r="H5" s="24">
         <v>29.501000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="2:26" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="I5" s="24">
+        <v>34.662999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>30</v>
       </c>
@@ -1761,8 +1844,10 @@
         <f>+D4-D5</f>
         <v>154.19499999999999</v>
       </c>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
+      <c r="E6" s="23">
+        <f>+E4-E5</f>
+        <v>181.113</v>
+      </c>
       <c r="G6" s="23">
         <f>+G4-G5</f>
         <v>215.34700000000004</v>
@@ -1771,6 +1856,10 @@
         <f>+H4-H5</f>
         <v>251.68300000000002</v>
       </c>
+      <c r="I6" s="23">
+        <f>+I4-I5</f>
+        <v>313.68799999999999</v>
+      </c>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
@@ -1783,6 +1872,9 @@
       <c r="D7" s="24">
         <v>109.726</v>
       </c>
+      <c r="E7" s="24">
+        <v>108.285</v>
+      </c>
       <c r="G7" s="24">
         <f>579.807-H7</f>
         <v>437.03000000000003</v>
@@ -1790,6 +1882,9 @@
       <c r="H7" s="24">
         <v>142.77699999999999</v>
       </c>
+      <c r="I7" s="24">
+        <v>166.70099999999999</v>
+      </c>
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
@@ -1802,6 +1897,9 @@
       <c r="D8" s="24">
         <v>59.225000000000001</v>
       </c>
+      <c r="E8" s="24">
+        <v>55.113999999999997</v>
+      </c>
       <c r="G8" s="24">
         <f>195.553-H8</f>
         <v>124.095</v>
@@ -1809,6 +1907,9 @@
       <c r="H8" s="24">
         <v>71.457999999999998</v>
       </c>
+      <c r="I8" s="24">
+        <v>74.510000000000005</v>
+      </c>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
@@ -1821,6 +1922,9 @@
       <c r="D9" s="24">
         <v>38.232999999999997</v>
       </c>
+      <c r="E9" s="24">
+        <v>37.228999999999999</v>
+      </c>
       <c r="G9" s="24">
         <f>311.964-H9</f>
         <v>243.477</v>
@@ -1828,8 +1932,11 @@
       <c r="H9" s="24">
         <v>68.486999999999995</v>
       </c>
-    </row>
-    <row r="10" spans="2:26" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="I9" s="24">
+        <v>65.653000000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>34</v>
       </c>
@@ -1841,8 +1948,10 @@
         <f>+D6-D7-D8-D9</f>
         <v>-52.989000000000004</v>
       </c>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
+      <c r="E10" s="23">
+        <f>+E6-E7-E8-E9</f>
+        <v>-19.514999999999993</v>
+      </c>
       <c r="G10" s="23">
         <f>+G6-G7-G8-G9</f>
         <v>-589.255</v>
@@ -1851,6 +1960,10 @@
         <f>+H6-H7-H8-H9</f>
         <v>-31.038999999999959</v>
       </c>
+      <c r="I10" s="23">
+        <f>+I6-I7-I8-I9</f>
+        <v>6.8239999999999839</v>
+      </c>
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
@@ -1863,6 +1976,9 @@
       <c r="D11" s="24">
         <v>13.305999999999999</v>
       </c>
+      <c r="E11" s="24">
+        <v>12.647</v>
+      </c>
       <c r="G11" s="24">
         <f>35.278-H11</f>
         <v>14.553999999999998</v>
@@ -1870,6 +1986,9 @@
       <c r="H11" s="24">
         <v>20.724</v>
       </c>
+      <c r="I11" s="24">
+        <v>22.968</v>
+      </c>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
@@ -1883,6 +2002,10 @@
         <f>+D10+D11</f>
         <v>-39.683000000000007</v>
       </c>
+      <c r="E12" s="24">
+        <f>+E10+E11</f>
+        <v>-6.8679999999999932</v>
+      </c>
       <c r="G12" s="24">
         <f>+G10+G11</f>
         <v>-574.70100000000002</v>
@@ -1891,6 +2014,10 @@
         <f>+H10+H11</f>
         <v>-10.314999999999959</v>
       </c>
+      <c r="I12" s="24">
+        <f>+I10+I11</f>
+        <v>29.791999999999984</v>
+      </c>
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
@@ -1903,6 +2030,9 @@
       <c r="D13" s="24">
         <v>1.4259999999999999</v>
       </c>
+      <c r="E13" s="24">
+        <v>0.44500000000000001</v>
+      </c>
       <c r="G13" s="24">
         <f>0.149-H13</f>
         <v>0.36499999999999999</v>
@@ -1910,8 +2040,11 @@
       <c r="H13" s="24">
         <v>-0.216</v>
       </c>
-    </row>
-    <row r="14" spans="2:26" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="I13" s="24">
+        <v>-3.1E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>37</v>
       </c>
@@ -1923,8 +2056,10 @@
         <f>+D12-D13</f>
         <v>-41.109000000000009</v>
       </c>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
+      <c r="E14" s="23">
+        <f>+E12-E13</f>
+        <v>-7.3129999999999935</v>
+      </c>
       <c r="G14" s="23">
         <f>+G12-G13</f>
         <v>-575.06600000000003</v>
@@ -1933,6 +2068,10 @@
         <f>+H12-H13</f>
         <v>-10.098999999999959</v>
       </c>
+      <c r="I14" s="23">
+        <f>+I12-I13</f>
+        <v>29.822999999999983</v>
+      </c>
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
@@ -1946,6 +2085,10 @@
         <f>+D14/D16</f>
         <v>-0.70261996626179901</v>
       </c>
+      <c r="E15" s="22">
+        <f>+E14/E16</f>
+        <v>-0.12425328034691817</v>
+      </c>
       <c r="G15" s="22">
         <f>+G14/G16</f>
         <v>-8.1871009673451596</v>
@@ -1954,6 +2097,10 @@
         <f>+H14/H16</f>
         <v>-6.1435891905339497E-2</v>
       </c>
+      <c r="I15" s="22">
+        <f>+I14/I16</f>
+        <v>0.17629020364506628</v>
+      </c>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
@@ -1965,17 +2112,20 @@
       <c r="D16" s="24">
         <v>58.508158000000002</v>
       </c>
+      <c r="E16" s="24">
+        <v>58.855589000000002</v>
+      </c>
       <c r="G16" s="24">
         <v>70.240492000000003</v>
       </c>
       <c r="H16" s="24">
         <v>164.38273599999999</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I16" s="24">
+        <v>169.16992200000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="25" t="s">
         <v>42</v>
       </c>
@@ -1987,8 +2137,10 @@
         <f>+D6/D4</f>
         <v>0.8424529178117367</v>
       </c>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
+      <c r="E18" s="25">
+        <f>+E6/E4</f>
+        <v>0.87280008481600702</v>
+      </c>
       <c r="G18" s="25">
         <f>+G6/G4</f>
         <v>0.88633660269259107</v>
@@ -1997,8 +2149,12 @@
         <f>+H6/H4</f>
         <v>0.89508293501763969</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I18" s="25">
+        <f>+I6/I4</f>
+        <v>0.90049404192897387</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="25" t="s">
         <v>43</v>
       </c>
@@ -2010,8 +2166,10 @@
         <f>D10/D4</f>
         <v>-0.28950833465369258</v>
       </c>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
+      <c r="E19" s="25">
+        <f>E10/E4</f>
+        <v>-9.4044566956454662E-2</v>
+      </c>
       <c r="G19" s="25">
         <f>G10/G4</f>
         <v>-2.4252869778525947</v>
@@ -2020,8 +2178,12 @@
         <f>H10/H4</f>
         <v>-0.11038679298964364</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I19" s="25">
+        <f>I10/I4</f>
+        <v>1.9589437090750374E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="25" t="s">
         <v>44</v>
       </c>
@@ -2033,8 +2195,10 @@
         <f>D14/D4</f>
         <v>-0.22460129704804108</v>
       </c>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58"/>
+      <c r="E20" s="25">
+        <f>E14/E4</f>
+        <v>-3.5242014765695745E-2</v>
+      </c>
       <c r="G20" s="25">
         <f>G14/G4</f>
         <v>-2.3668871391940334</v>
@@ -2043,8 +2207,12 @@
         <f>H14/H4</f>
         <v>-3.591598383976314E-2</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I20" s="25">
+        <f>I14/I4</f>
+        <v>8.5611925902322611E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="25" t="s">
         <v>39</v>
       </c>
@@ -2056,8 +2224,10 @@
         <f>D13/D12</f>
         <v>-3.5934783156515375E-2</v>
       </c>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
+      <c r="E21" s="25">
+        <f>E13/E12</f>
+        <v>-6.4793244030285441E-2</v>
+      </c>
       <c r="G21" s="25">
         <f>G13/G12</f>
         <v>-6.3511286738669325E-4</v>
@@ -2066,22 +2236,26 @@
         <f>H13/H12</f>
         <v>2.0940378090160045E-2</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" s="26" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I21" s="25">
+        <f>I13/I12</f>
+        <v>-1.0405477980665956E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" s="53" t="s">
-        <v>94</v>
+      <c r="C24" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="43" t="s">
+        <v>93</v>
       </c>
       <c r="G24" s="26">
         <f>G4/C4-1</f>
@@ -2091,31 +2265,37 @@
         <f>H4/D4-1</f>
         <v>0.53626434866224848</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I24" s="26">
+        <f t="shared" ref="I24" si="0">I4/E4-1</f>
+        <v>0.67873527767604136</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="53" t="s">
-        <v>94</v>
+      <c r="C25" s="43" t="s">
+        <v>93</v>
       </c>
       <c r="D25" s="25">
         <f>D4/C4-1</f>
         <v>0.1178148283864664</v>
       </c>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
       <c r="H25" s="25">
         <f>H4/G4-1</f>
         <v>0.15731201870243616</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="25">
+        <f t="shared" ref="I25" si="1">I4/H4-1</f>
+        <v>0.23887205530897915</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="27" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" s="24" customFormat="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B28" s="24" t="s">
         <v>16</v>
       </c>
@@ -2127,11 +2307,11 @@
         <f>32.1+28.3</f>
         <v>60.400000000000006</v>
       </c>
-      <c r="E28" s="59">
+      <c r="E28" s="24">
         <f>34.7+31.3</f>
         <v>66</v>
       </c>
-      <c r="F28" s="59">
+      <c r="F28" s="24">
         <f>36.4+36.7</f>
         <v>73.099999999999994</v>
       </c>
@@ -2142,13 +2322,14 @@
       <c r="H28" s="24">
         <v>91.2</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I28" s="24">
+        <v>97.2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" s="40" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B29" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
+        <v>87</v>
+      </c>
       <c r="G29" s="41">
         <f>G28/C28-1</f>
         <v>0.37147595356550589</v>
@@ -2157,462 +2338,652 @@
         <f>H28/D28-1</f>
         <v>0.50993377483443703</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="41">
+        <f>I28/E28-1</f>
+        <v>0.47272727272727266</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H30" s="1">
         <v>3.08</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="1">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="38" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" s="27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="M33" s="24">
+        <v>1383</v>
+      </c>
+      <c r="N33" s="24">
+        <v>1942</v>
+      </c>
+      <c r="O33" s="24">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="N34" s="25">
+        <f>N33/M33-1</f>
+        <v>0.40419378163412878</v>
+      </c>
+      <c r="O34" s="25">
+        <f>O33/N33-1</f>
+        <v>3.6560247167868098E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B35" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B36" s="27"/>
+    </row>
+    <row r="37" spans="2:15" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="23">
+        <v>401.17599999999999</v>
+      </c>
+      <c r="G37" s="23">
+        <v>968.51499999999999</v>
+      </c>
+      <c r="H37" s="23">
+        <v>467.952</v>
+      </c>
+      <c r="I37" s="23">
+        <v>515.89499999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="56"/>
-      <c r="F35" s="61">
-        <v>401.17599999999999</v>
-      </c>
-      <c r="G35" s="23">
-        <v>968.51499999999999</v>
-      </c>
-      <c r="H35" s="23">
-        <v>467.952</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
+      <c r="F38" s="23">
+        <v>811.94600000000003</v>
+      </c>
+      <c r="G38" s="23">
+        <v>701.83500000000004</v>
+      </c>
+      <c r="H38" s="23">
+        <v>1231.0989999999999</v>
+      </c>
+      <c r="I38" s="23">
+        <v>1229.0719999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="56"/>
-      <c r="F36" s="61">
-        <v>811.94600000000003</v>
-      </c>
-      <c r="G36" s="23">
-        <v>701.83500000000004</v>
-      </c>
-      <c r="H36" s="23">
-        <v>1231.0989999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
+      <c r="F39" s="24">
+        <v>245.279</v>
+      </c>
+      <c r="G39" s="24">
+        <v>215.30699999999999</v>
+      </c>
+      <c r="H39" s="24">
+        <v>240.09299999999999</v>
+      </c>
+      <c r="I39" s="24">
+        <v>283.89</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F37" s="59">
-        <v>245.279</v>
-      </c>
-      <c r="G37" s="24">
-        <v>215.30699999999999</v>
-      </c>
-      <c r="H37" s="24">
-        <v>240.09299999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
+      <c r="F40" s="24">
+        <v>21.286000000000001</v>
+      </c>
+      <c r="G40" s="24">
+        <v>34.368000000000002</v>
+      </c>
+      <c r="H40" s="24">
+        <v>41.598999999999997</v>
+      </c>
+      <c r="I40" s="24">
+        <v>31.974</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F38" s="59">
-        <v>21.286000000000001</v>
-      </c>
-      <c r="G38" s="24">
-        <v>34.368000000000002</v>
-      </c>
-      <c r="H38" s="24">
-        <v>41.598999999999997</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
+      <c r="F41" s="24">
+        <f>SUM(F37:F40)</f>
+        <v>1479.6870000000001</v>
+      </c>
+      <c r="G41" s="24">
+        <f>SUM(G37:G40)</f>
+        <v>1920.0249999999999</v>
+      </c>
+      <c r="H41" s="24">
+        <f>SUM(H37:H40)</f>
+        <v>1980.7429999999999</v>
+      </c>
+      <c r="I41" s="24">
+        <f>SUM(I37:I40)</f>
+        <v>2060.8310000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F39" s="24">
-        <f>SUM(F35:F38)</f>
-        <v>1479.6870000000001</v>
-      </c>
-      <c r="G39" s="24">
-        <f>SUM(G35:G38)</f>
-        <v>1920.0249999999999</v>
-      </c>
-      <c r="H39" s="24">
-        <f>SUM(H35:H38)</f>
-        <v>1980.7429999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
+      <c r="F42" s="24">
+        <v>14.946</v>
+      </c>
+      <c r="G42" s="24">
+        <v>14.385</v>
+      </c>
+      <c r="H42" s="24">
+        <v>14.167999999999999</v>
+      </c>
+      <c r="I42" s="24">
+        <v>13.775</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F40" s="59">
-        <v>14.946</v>
-      </c>
-      <c r="G40" s="24">
-        <v>14.385</v>
-      </c>
-      <c r="H40" s="24">
-        <v>14.167999999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
+      <c r="F43" s="24">
+        <v>24.007999999999999</v>
+      </c>
+      <c r="G43" s="24">
+        <v>22.754000000000001</v>
+      </c>
+      <c r="H43" s="24">
+        <v>25.106999999999999</v>
+      </c>
+      <c r="I43" s="24">
+        <v>23.872</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F41" s="59">
-        <v>24.007999999999999</v>
-      </c>
-      <c r="G41" s="24">
-        <v>22.754000000000001</v>
-      </c>
-      <c r="H41" s="24">
-        <v>25.106999999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F42" s="59">
+      <c r="F44" s="24">
         <f>32.147+26.299</f>
         <v>58.445999999999998</v>
       </c>
-      <c r="G42" s="24">
+      <c r="G44" s="24">
         <f>26.299+29.928</f>
         <v>56.227000000000004</v>
       </c>
-      <c r="H42" s="24">
+      <c r="H44" s="24">
         <f>27.772+26.299</f>
         <v>54.070999999999998</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
+      <c r="I44" s="24">
+        <f>27.904+42.174</f>
+        <v>70.078000000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F45" s="24">
+        <v>19.38</v>
+      </c>
+      <c r="G45" s="24">
+        <v>2.5049999999999999</v>
+      </c>
+      <c r="H45" s="24">
+        <v>2.2730000000000001</v>
+      </c>
+      <c r="I45" s="24">
+        <v>3.1520000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F43" s="59">
-        <v>19.38</v>
-      </c>
-      <c r="G43" s="24">
-        <v>2.5049999999999999</v>
-      </c>
-      <c r="H43" s="24">
-        <v>2.2730000000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
+      <c r="F46" s="24">
+        <f>SUM(F41:F45)</f>
+        <v>1596.4670000000001</v>
+      </c>
+      <c r="G46" s="24">
+        <f>SUM(G41:G45)</f>
+        <v>2015.896</v>
+      </c>
+      <c r="H46" s="24">
+        <f>SUM(H41:H45)</f>
+        <v>2076.3620000000001</v>
+      </c>
+      <c r="I46" s="24">
+        <f>SUM(I41:I45)</f>
+        <v>2171.7080000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F44" s="24">
-        <f>SUM(F39:F43)</f>
-        <v>1596.4670000000001</v>
-      </c>
-      <c r="G44" s="24">
-        <f>SUM(G39:G43)</f>
-        <v>2015.896</v>
-      </c>
-      <c r="H44" s="24">
-        <f>SUM(H39:H43)</f>
-        <v>2076.3620000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
+      <c r="F48" s="24">
+        <v>46.514000000000003</v>
+      </c>
+      <c r="G48" s="28">
+        <v>45.378</v>
+      </c>
+      <c r="H48" s="24">
+        <v>64.328999999999994</v>
+      </c>
+      <c r="I48" s="24">
+        <v>62.042000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F46" s="59">
-        <v>46.514000000000003</v>
-      </c>
-      <c r="G46" s="28">
-        <v>45.378</v>
-      </c>
-      <c r="H46" s="24">
-        <v>64.328999999999994</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F47" s="59">
+      <c r="F49" s="24">
         <v>3.7069999999999999</v>
       </c>
-      <c r="G47" s="28">
+      <c r="G49" s="28">
         <v>4.383</v>
       </c>
-      <c r="H47" s="24">
+      <c r="H49" s="24">
         <v>5.3680000000000003</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B48" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F48" s="59">
-        <v>83.349000000000004</v>
-      </c>
-      <c r="G48" s="28">
-        <v>106.724</v>
-      </c>
-      <c r="H48" s="24">
-        <v>89.817999999999998</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F49" s="24">
-        <f>SUM(F46:F48)</f>
-        <v>133.57</v>
-      </c>
-      <c r="G49" s="28">
-        <f>SUM(G46:G48)</f>
-        <v>156.48500000000001</v>
-      </c>
-      <c r="H49" s="24">
-        <f>SUM(H46:H48)</f>
-        <v>159.51499999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I49" s="24">
+        <v>5.3979999999999997</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F50" s="59">
+      <c r="F50" s="24">
+        <v>83.349000000000004</v>
+      </c>
+      <c r="G50" s="28">
+        <v>106.724</v>
+      </c>
+      <c r="H50" s="24">
+        <v>89.817999999999998</v>
+      </c>
+      <c r="I50" s="24">
+        <v>104.84399999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F51" s="24">
+        <f>SUM(F48:F50)</f>
+        <v>133.57</v>
+      </c>
+      <c r="G51" s="28">
+        <f>SUM(G48:G50)</f>
+        <v>156.48500000000001</v>
+      </c>
+      <c r="H51" s="24">
+        <f>SUM(H48:H50)</f>
+        <v>159.51499999999999</v>
+      </c>
+      <c r="I51" s="24">
+        <f>SUM(I48:I50)</f>
+        <v>172.28399999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F52" s="24">
         <v>22.04</v>
       </c>
-      <c r="G50" s="28">
+      <c r="G52" s="28">
         <v>20.835000000000001</v>
       </c>
-      <c r="H50" s="24">
+      <c r="H52" s="24">
         <v>22.757000000000001</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B51" s="1" t="s">
+      <c r="I52" s="24">
+        <v>21.567</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F53" s="24">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="G53" s="28">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="H53" s="24">
+        <v>0.255</v>
+      </c>
+      <c r="I53" s="24">
+        <v>0.249</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B54" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F54" s="24">
+        <f>SUM(F51:F53)</f>
+        <v>155.89699999999999</v>
+      </c>
+      <c r="G54" s="28">
+        <f>SUM(G51:G53)</f>
+        <v>177.59600000000003</v>
+      </c>
+      <c r="H54" s="24">
+        <f>SUM(H51:H53)</f>
+        <v>182.52699999999999</v>
+      </c>
+      <c r="I54" s="24">
+        <f>SUM(I51:I53)</f>
+        <v>194.1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F51" s="59">
-        <v>0.28699999999999998</v>
-      </c>
-      <c r="G51" s="28">
-        <v>0.27600000000000002</v>
-      </c>
-      <c r="H51" s="24">
-        <v>0.255</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B52" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F52" s="24">
-        <f>SUM(F49:F51)</f>
-        <v>155.89699999999999</v>
-      </c>
-      <c r="G52" s="28">
-        <f>SUM(G49:G51)</f>
-        <v>177.59600000000003</v>
-      </c>
-      <c r="H52" s="24">
-        <f>SUM(H49:H51)</f>
-        <v>182.52699999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="24" t="s">
+      <c r="F56" s="24">
+        <f>+F46-F54</f>
+        <v>1440.5700000000002</v>
+      </c>
+      <c r="G56" s="24">
+        <v>1838.3</v>
+      </c>
+      <c r="H56" s="24">
+        <v>1893.835</v>
+      </c>
+      <c r="I56" s="24">
+        <v>1977.6079999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E54" s="59"/>
-      <c r="F54" s="59">
-        <f>+F44-F52</f>
+      <c r="F57" s="24">
+        <f>+F56+F54</f>
+        <v>1596.4670000000001</v>
+      </c>
+      <c r="G57" s="24">
+        <f>+G56+G54</f>
+        <v>2015.896</v>
+      </c>
+      <c r="H57" s="24">
+        <f>+H56+H54</f>
+        <v>2076.3620000000001</v>
+      </c>
+      <c r="I57" s="24">
+        <f>+I56+I54</f>
+        <v>2171.7080000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B59" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F59" s="24">
+        <f>+F46-F54</f>
         <v>1440.5700000000002</v>
       </c>
-      <c r="G54" s="24">
+      <c r="G59" s="24">
+        <f>+G46-G54</f>
         <v>1838.3</v>
       </c>
-      <c r="H54" s="24">
+      <c r="H59" s="24">
+        <f>+H46-H54</f>
         <v>1893.835</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F55" s="24">
-        <f>+F54+F52</f>
-        <v>1596.4670000000001</v>
-      </c>
-      <c r="G55" s="24">
-        <f>+G54+G52</f>
-        <v>2015.896</v>
-      </c>
-      <c r="H55" s="24">
-        <f>+H54+H52</f>
-        <v>2076.3620000000001</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="1" t="s">
+      <c r="I59" s="24">
+        <f>+I46-I54</f>
+        <v>1977.6080000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B60" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F57" s="24">
-        <f>+F44-F52</f>
-        <v>1440.5700000000002</v>
-      </c>
-      <c r="G57" s="24">
-        <f>+G44-G52</f>
-        <v>1838.3</v>
-      </c>
-      <c r="H57" s="24">
-        <f>+H44-H52</f>
-        <v>1893.835</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B58" s="1" t="s">
+      <c r="G60" s="1">
+        <f>G59/G16</f>
+        <v>26.17151371889593</v>
+      </c>
+      <c r="H60" s="1">
+        <f>H59/H16</f>
+        <v>11.520887448910694</v>
+      </c>
+      <c r="I60" s="1">
+        <f>I59/I16</f>
+        <v>11.69006863997963</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" s="24">
+        <f>+F37+F38</f>
+        <v>1213.1220000000001</v>
+      </c>
+      <c r="G62" s="24">
+        <f>+G37+G38</f>
+        <v>1670.35</v>
+      </c>
+      <c r="H62" s="24">
+        <f>+H37+H38</f>
+        <v>1699.0509999999999</v>
+      </c>
+      <c r="I62" s="24">
+        <f>+I37+I38</f>
+        <v>1744.9669999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" s="24">
+        <f>+F62-F63</f>
+        <v>1213.1220000000001</v>
+      </c>
+      <c r="G64" s="24">
+        <f>+G62-G63</f>
+        <v>1670.35</v>
+      </c>
+      <c r="H64" s="24">
+        <f>+H62-H63</f>
+        <v>1699.0509999999999</v>
+      </c>
+      <c r="I64" s="24">
+        <f>+I62-I63</f>
+        <v>1744.9669999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B66" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1">
-        <f>G57/G16</f>
-        <v>26.17151371889593</v>
-      </c>
-      <c r="H58" s="1">
-        <f>H57/H16</f>
-        <v>11.520887448910694</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F60" s="24">
-        <f>+F35+F36</f>
-        <v>1213.1220000000001</v>
-      </c>
-      <c r="G60" s="24">
-        <f>+G35+G36</f>
-        <v>1670.35</v>
-      </c>
-      <c r="H60" s="24">
-        <f>+H35+H36</f>
-        <v>1699.0509999999999</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B61" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F61" s="1">
-        <v>0</v>
-      </c>
-      <c r="G61" s="1">
-        <v>0</v>
-      </c>
-      <c r="H61" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F62" s="24">
-        <f>+F60-F61</f>
-        <v>1213.1220000000001</v>
-      </c>
-      <c r="G62" s="24">
-        <f>+G60-G61</f>
-        <v>1670.35</v>
-      </c>
-      <c r="H62" s="24">
-        <f>+H60-H61</f>
-        <v>1699.0509999999999</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B64" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B65" s="1" t="s">
+      <c r="G66" s="1">
+        <v>49.92</v>
+      </c>
+      <c r="H66" s="1">
+        <v>63.58</v>
+      </c>
+      <c r="I66" s="1">
+        <v>81.739999999999995</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="24" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B66" s="1" t="s">
+      <c r="G67" s="24">
+        <f>+G66*G16</f>
+        <v>3506.4053606400003</v>
+      </c>
+      <c r="H67" s="24">
+        <f>+H66*H16</f>
+        <v>10451.454354879999</v>
+      </c>
+      <c r="I67" s="24">
+        <f>+I66*I16</f>
+        <v>13827.949424280001</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B68" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B70" s="27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B71" s="1" t="s">
+      <c r="G68" s="24">
+        <f>+G67-G64</f>
+        <v>1836.0553606400003</v>
+      </c>
+      <c r="H68" s="24">
+        <f>+H67-H64</f>
+        <v>8752.4033548799998</v>
+      </c>
+      <c r="I68" s="24">
+        <f>+I67-I64</f>
+        <v>12082.98242428</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B72" s="27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B73" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D73" s="24"/>
+      <c r="F73" s="24">
+        <v>4.0750000000000002</v>
+      </c>
+      <c r="G73" s="24">
+        <v>32.064</v>
+      </c>
+      <c r="H73" s="28">
+        <v>28.385000000000002</v>
+      </c>
+      <c r="I73" s="28">
+        <v>71.622</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B74" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F71" s="59">
-        <v>4.0750000000000002</v>
-      </c>
-      <c r="G71" s="24">
-        <v>32.064</v>
-      </c>
-      <c r="H71" s="28">
-        <v>28.385000000000002</v>
-      </c>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B72" s="1" t="s">
+      <c r="D74" s="24"/>
+      <c r="F74" s="24">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="G74" s="24">
+        <v>2.851</v>
+      </c>
+      <c r="H74" s="28">
+        <v>1.202</v>
+      </c>
+      <c r="I74" s="28">
+        <v>1.353</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F72" s="59">
-        <v>0.35599999999999998</v>
-      </c>
-      <c r="G72" s="24">
-        <v>2.851</v>
-      </c>
-      <c r="H72" s="28">
-        <v>1.202</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B73" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F73" s="28">
-        <f>+F71-F72</f>
+      <c r="D75" s="56"/>
+      <c r="F75" s="56">
+        <f>+F73-F74</f>
         <v>3.7190000000000003</v>
       </c>
-      <c r="G73" s="28">
-        <f>+G71-G72</f>
+      <c r="G75" s="56">
+        <f>+G73-G74</f>
         <v>29.213000000000001</v>
       </c>
-      <c r="H73" s="28">
-        <f>+H71-H72</f>
+      <c r="H75" s="56">
+        <f>+H73-H74</f>
         <v>27.183</v>
+      </c>
+      <c r="I75" s="56">
+        <f>+I73-I74</f>
+        <v>70.269000000000005</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B76" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I76" s="28">
+        <f>+SUM(F75:I75)</f>
+        <v>130.38400000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B77" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I77" s="1">
+        <f>+I76/I16</f>
+        <v>0.77072802575389265</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B79" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I79" s="1">
+        <f>+I66/I77</f>
+        <v>106.05556988802306</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H1" r:id="rId1" xr:uid="{E02EB090-7FBE-4B92-AEB7-694A4D3430AF}"/>
     <hyperlink ref="G1" r:id="rId2" xr:uid="{89CF086C-830A-4261-A715-CBE0EE96DCF3}"/>
+    <hyperlink ref="I1" r:id="rId3" xr:uid="{7BC3322F-073F-4C18-AA86-42BA9300B990}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>